<commit_message>
submit the excel test file
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/student.xlsx
+++ b/src/main/resources/templates/student.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9060"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>学号</t>
   </si>
@@ -46,6 +46,9 @@
     <t>出生日期</t>
   </si>
   <si>
+    <t>入学日期(需设置单元格格式)</t>
+  </si>
+  <si>
     <t xml:space="preserve">S001 </t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>男</t>
+  </si>
+  <si>
+    <t>2022-0-01</t>
   </si>
   <si>
     <t xml:space="preserve">S002 </t>
@@ -74,25 +80,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="[$-409]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.45"/>
-      <color rgb="FF494949"/>
-      <name val="Courier New"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -559,133 +560,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -693,10 +694,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1010,18 +1011,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="5" max="5" width="9.66666666666667"/>
+    <col min="5" max="5" width="11.5" style="1"/>
+    <col min="6" max="6" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1034,19 +1036,22 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>13</v>
@@ -1054,39 +1059,48 @@
       <c r="E2" s="1">
         <v>44805</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>14</v>
       </c>
       <c r="E3" s="1">
-        <v>44805</v>
+        <v>44806</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
       <c r="D4">
         <v>15</v>
       </c>
-      <c r="E4" s="2">
-        <v>44805</v>
+      <c r="E4" s="1">
+        <v>44807</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1119,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1122,7 +1136,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>